<commit_message>
Updated all relevant documentation files to include License and Acknowledgements.  Minor tweaks to assembly descriptors
git-svn-id: svn://svn.code.sf.net/p/sparql-query-bm/code/trunk@8 37c29ba0-d37e-4076-90e9-b7b408e7d1da
</commit_message>
<xml_diff>
--- a/documents/reports/semtech2012/SemTech 2012 Results.xlsx
+++ b/documents/reports/semtech2012/SemTech 2012 Results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28280" windowHeight="18000" tabRatio="500" firstSheet="20" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28280" windowHeight="18000" tabRatio="500" firstSheet="14" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TDB 10k" sheetId="2" r:id="rId1"/>
@@ -981,11 +981,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2069854584"/>
-        <c:axId val="2069861432"/>
+        <c:axId val="2144983768"/>
+        <c:axId val="2142994184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069854584"/>
+        <c:axId val="2144983768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069861432"/>
+        <c:crossAx val="2142994184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069861432"/>
+        <c:axId val="2142994184"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1052,7 +1052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069854584"/>
+        <c:crossAx val="2144983768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1356,11 +1356,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2146820264"/>
-        <c:axId val="2146814776"/>
+        <c:axId val="2140362648"/>
+        <c:axId val="2140357144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2146820264"/>
+        <c:axId val="2140362648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1388,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146814776"/>
+        <c:crossAx val="2140357144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1396,7 +1396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146814776"/>
+        <c:axId val="2140357144"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1432,7 +1432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146820264"/>
+        <c:crossAx val="2140362648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1744,11 +1744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2146770088"/>
-        <c:axId val="2146764600"/>
+        <c:axId val="2140307272"/>
+        <c:axId val="2140301768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2146770088"/>
+        <c:axId val="2140307272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +1776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146764600"/>
+        <c:crossAx val="2140301768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1784,7 +1784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146764600"/>
+        <c:axId val="2140301768"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1815,7 +1815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146770088"/>
+        <c:crossAx val="2140307272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2067,11 +2067,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131794056"/>
-        <c:axId val="-2131788616"/>
+        <c:axId val="2144160168"/>
+        <c:axId val="2144165656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131794056"/>
+        <c:axId val="2144160168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131788616"/>
+        <c:crossAx val="2144165656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2107,7 +2107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131788616"/>
+        <c:axId val="2144165656"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2138,7 +2138,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131794056"/>
+        <c:crossAx val="2144160168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2390,11 +2390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2132341800"/>
-        <c:axId val="-2132347304"/>
+        <c:axId val="2144212216"/>
+        <c:axId val="2144217704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2132341800"/>
+        <c:axId val="2144212216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +2422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132347304"/>
+        <c:crossAx val="2144217704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2430,7 +2430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132347304"/>
+        <c:axId val="2144217704"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2466,7 +2466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132341800"/>
+        <c:crossAx val="2144212216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,11 +2726,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2132406024"/>
-        <c:axId val="-2132411480"/>
+        <c:axId val="2144263448"/>
+        <c:axId val="2144268936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2132406024"/>
+        <c:axId val="2144263448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2758,7 +2758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132411480"/>
+        <c:crossAx val="2144268936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2766,7 +2766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132411480"/>
+        <c:axId val="2144268936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2797,7 +2797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132406024"/>
+        <c:crossAx val="2144263448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3484,11 +3484,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144562360"/>
-        <c:axId val="-2144559384"/>
+        <c:axId val="2143762248"/>
+        <c:axId val="2143759256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144562360"/>
+        <c:axId val="2143762248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3497,7 +3497,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144559384"/>
+        <c:crossAx val="2143759256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3505,7 +3505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144559384"/>
+        <c:axId val="2143759256"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3513,11 +3513,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Runtime in Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144562360"/>
+        <c:crossAx val="2143762248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4068,11 +4087,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127974936"/>
-        <c:axId val="-2127971960"/>
+        <c:axId val="2143703064"/>
+        <c:axId val="2143699912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127974936"/>
+        <c:axId val="2143703064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4081,7 +4100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127971960"/>
+        <c:crossAx val="2143699912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4089,7 +4108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127971960"/>
+        <c:axId val="2143699912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4101,7 +4120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127974936"/>
+        <c:crossAx val="2143703064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22326,8 +22345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23530,8 +23549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="S48" sqref="S48"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23550,7 +23569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>

</xml_diff>